<commit_message>
Implemented category printing feature
</commit_message>
<xml_diff>
--- a/Kategorien.xlsx
+++ b/Kategorien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\SV-Tora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E3BED5-A44C-46C7-898E-4E75EA2E62BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14626E7A-F05E-4E13-96DA-F9E2C40E0C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="61656" windowHeight="16776" xr2:uid="{85CA4AFD-A916-4224-BE1D-5C85425191EB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85CA4AFD-A916-4224-BE1D-5C85425191EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
   <si>
     <t>Kihon</t>
   </si>
@@ -262,13 +262,16 @@
   </si>
   <si>
     <t>48</t>
+  </si>
+  <si>
+    <t>Kategorien</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,6 +300,12 @@
       <name val="Baloo Chettan 2"/>
       <family val="4"/>
     </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Baloo Chettan 2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -684,10 +693,67 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -702,64 +768,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1076,533 +1085,555 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B2A268-E397-44A7-B559-AAE7BD59F659}">
-  <dimension ref="A2:K38"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19.8" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="11.5546875" style="2"/>
+    <col min="1" max="1" width="1.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="2"/>
     <col min="3" max="3" width="15.109375" style="2" customWidth="1"/>
     <col min="4" max="5" width="11.109375" style="2" customWidth="1"/>
     <col min="6" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="25.8" x14ac:dyDescent="0.7">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:11" ht="33" customHeight="1">
+      <c r="B2" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+    </row>
+    <row r="4" spans="2:11" ht="21">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="9"/>
-      <c r="C3" s="10" t="s">
+    <row r="5" spans="2:11" ht="15.6">
+      <c r="B5" s="9"/>
+      <c r="C5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="40"/>
-    </row>
-    <row r="4" spans="2:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B4" s="11" t="s">
+      <c r="E5" s="37"/>
+    </row>
+    <row r="6" spans="2:11" ht="16.2" thickBot="1">
+      <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E6" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="13" t="s">
+    <row r="7" spans="2:11">
+      <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="8" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="14" t="s">
+    <row r="8" spans="2:11">
+      <c r="B8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16" t="s">
+      <c r="C8" s="15"/>
+      <c r="D8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E8" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="25.8" x14ac:dyDescent="0.7">
-      <c r="B9" s="1" t="s">
+    <row r="11" spans="2:11" ht="21">
+      <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10" t="s">
+    <row r="12" spans="2:11" ht="15.6">
+      <c r="B12" s="9"/>
+      <c r="C12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D12" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="40"/>
-    </row>
-    <row r="11" spans="2:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B11" s="11" t="s">
+      <c r="E12" s="37"/>
+    </row>
+    <row r="13" spans="2:11" ht="16.2" thickBot="1">
+      <c r="B13" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E13" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="13" t="s">
+    <row r="14" spans="2:11">
+      <c r="B14" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="8" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="13" t="s">
+    <row r="15" spans="2:11">
+      <c r="B15" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="8" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E15" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="14" t="s">
+    <row r="16" spans="2:11">
+      <c r="B16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="18" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E16" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="9"/>
-      <c r="C16" s="10" t="s">
+    <row r="17" spans="2:11">
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="2:11" ht="15.6">
+      <c r="B18" s="9"/>
+      <c r="C18" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D18" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="33" t="s">
+      <c r="E18" s="37"/>
+      <c r="F18" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="40"/>
-    </row>
-    <row r="17" spans="2:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B17" s="11" t="s">
+      <c r="G18" s="37"/>
+    </row>
+    <row r="19" spans="2:11" ht="16.2" thickBot="1">
+      <c r="B19" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D19" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E19" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="F19" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G19" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="13" t="s">
+    <row r="20" spans="2:11">
+      <c r="B20" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="13" t="s">
-        <v>30</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11">
+      <c r="B21" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11">
+      <c r="B22" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E22" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="F22" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G22" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="14" t="s">
+    <row r="23" spans="2:11">
+      <c r="B23" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="18" t="s">
+      <c r="C23" s="15"/>
+      <c r="D23" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E23" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="35" t="s">
+      <c r="F23" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="G23" s="19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="25.8" x14ac:dyDescent="0.7">
-      <c r="B24" s="1" t="s">
+    <row r="26" spans="2:11" ht="21">
+      <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B25" s="26" t="s">
+    <row r="27" spans="2:11" ht="16.2" thickBot="1">
+      <c r="B27" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="21" t="s">
+      <c r="C27" s="21"/>
+      <c r="D27" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="20"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B26" s="13" t="s">
+      <c r="E27" s="42"/>
+    </row>
+    <row r="28" spans="2:11">
+      <c r="B28" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="22" t="s">
+      <c r="C28" s="5"/>
+      <c r="D28" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="23"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" s="14" t="s">
+      <c r="E28" s="44"/>
+    </row>
+    <row r="29" spans="2:11">
+      <c r="B29" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="24" t="s">
+      <c r="C29" s="15"/>
+      <c r="D29" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="25"/>
-    </row>
-    <row r="30" spans="2:11" ht="25.8" x14ac:dyDescent="0.7">
-      <c r="B30" s="1" t="s">
+      <c r="E29" s="46"/>
+    </row>
+    <row r="32" spans="2:11" ht="21">
+      <c r="B32" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B31" s="9"/>
-      <c r="C31" s="10" t="s">
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+    </row>
+    <row r="33" spans="1:11" ht="15.6">
+      <c r="B33" s="9"/>
+      <c r="C33" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="39" t="s">
+      <c r="D33" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="29" t="s">
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="I31" s="28"/>
-      <c r="J31" s="43" t="s">
+      <c r="I33" s="37"/>
+      <c r="J33" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="K31" s="30"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B32" s="31"/>
-      <c r="C32" s="3" t="s">
+      <c r="K33" s="28"/>
+    </row>
+    <row r="34" spans="1:11" ht="15.6">
+      <c r="B34" s="22"/>
+      <c r="C34" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="41" t="s">
+      <c r="D34" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="30"/>
-      <c r="F32" s="29" t="s">
+      <c r="E34" s="28"/>
+      <c r="F34" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="G32" s="30"/>
-      <c r="H32" s="29" t="s">
+      <c r="G34" s="28"/>
+      <c r="H34" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="I32" s="30"/>
-      <c r="J32" s="43" t="s">
+      <c r="I34" s="28"/>
+      <c r="J34" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="K32" s="30"/>
-    </row>
-    <row r="33" spans="1:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B33" s="11" t="s">
+      <c r="K34" s="28"/>
+    </row>
+    <row r="35" spans="1:11" ht="16.2" thickBot="1">
+      <c r="B35" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D35" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E35" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="44" t="s">
+      <c r="F35" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="G33" s="45"/>
-      <c r="H33" s="42" t="s">
+      <c r="G35" s="33"/>
+      <c r="H35" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="I33" s="12" t="s">
+      <c r="I35" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J33" s="42" t="s">
+      <c r="J35" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="K33" s="12" t="s">
+      <c r="K35" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B34" s="13" t="s">
+    <row r="36" spans="1:11">
+      <c r="B36" s="13" t="s">
         <v>7</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F34" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="G34" s="47"/>
-      <c r="H34" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="J34" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="K34" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B35" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F35" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="G35" s="30"/>
-      <c r="H35" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="J35" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="K35" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B36" s="13" t="s">
-        <v>15</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G36" s="35"/>
+      <c r="H36" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J36" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="B37" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F37" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" s="28"/>
+      <c r="H37" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J37" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="B38" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E38" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F36" s="29" t="s">
+      <c r="F38" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="G36" s="30"/>
-      <c r="H36" s="34" t="s">
+      <c r="G38" s="28"/>
+      <c r="H38" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="I36" s="7" t="s">
+      <c r="I38" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J36" s="34" t="s">
+      <c r="J38" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="K36" s="7" t="s">
+      <c r="K38" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B37" s="13" t="s">
+    <row r="39" spans="1:11">
+      <c r="B39" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="7" t="s">
+      <c r="C39" s="5"/>
+      <c r="D39" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E37" s="34" t="s">
+      <c r="E39" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="F37" s="29" t="s">
+      <c r="F39" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="G37" s="30"/>
-      <c r="H37" s="34" t="s">
+      <c r="G39" s="28"/>
+      <c r="H39" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="I37" s="7" t="s">
+      <c r="I39" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J37" s="34" t="s">
+      <c r="J39" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="K37" s="7" t="s">
+      <c r="K39" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="6"/>
-      <c r="B38" s="14" t="s">
+    <row r="40" spans="1:11">
+      <c r="A40" s="6"/>
+      <c r="B40" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="18" t="s">
+      <c r="C40" s="15"/>
+      <c r="D40" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="35" t="s">
+      <c r="E40" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="F38" s="38" t="s">
+      <c r="F40" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="G38" s="37"/>
-      <c r="H38" s="35" t="s">
+      <c r="G40" s="30"/>
+      <c r="H40" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="I38" s="19" t="s">
+      <c r="I40" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="J38" s="35" t="s">
+      <c r="J40" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="K38" s="19" t="s">
+      <c r="K40" s="19" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="21">
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="H33:I33"/>
     <mergeCell ref="F35:G35"/>
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="F37:G37"/>
     <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H34:I34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="72" orientation="portrait" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="41" max="16383" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix: Fixed a bunch of bugs and implemented final wanted changes by product owners
</commit_message>
<xml_diff>
--- a/Kategorien.xlsx
+++ b/Kategorien.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\SV-Tora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14626E7A-F05E-4E13-96DA-F9E2C40E0C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB63DE54-A6BF-4C3E-B5C8-7145C96A2883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85CA4AFD-A916-4224-BE1D-5C85425191EB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="61656" windowHeight="16776" xr2:uid="{85CA4AFD-A916-4224-BE1D-5C85425191EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="99">
   <si>
     <t>Kihon</t>
   </si>
@@ -114,12 +114,6 @@
     <t>m/w</t>
   </si>
   <si>
-    <t>8-11</t>
-  </si>
-  <si>
-    <t>12-17</t>
-  </si>
-  <si>
     <t>7. - 6. Kyu</t>
   </si>
   <si>
@@ -265,6 +259,78 @@
   </si>
   <si>
     <t>Kategorien</t>
+  </si>
+  <si>
+    <t>18-20</t>
+  </si>
+  <si>
+    <t>ab 21</t>
+  </si>
+  <si>
+    <t>8-12</t>
+  </si>
+  <si>
+    <t>13-20</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
   </si>
 </sst>
 </file>
@@ -656,7 +722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -714,25 +780,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -742,6 +790,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -768,7 +822,25 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1088,10 +1160,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K40"/>
+  <dimension ref="A2:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1104,18 +1176,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="33" customHeight="1">
-      <c r="B2" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
+      <c r="B2" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
     </row>
     <row r="4" spans="2:11" ht="21">
       <c r="B4" s="1" t="s">
@@ -1127,10 +1199,10 @@
       <c r="C5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="37"/>
+      <c r="E5" s="31"/>
     </row>
     <row r="6" spans="2:11" ht="16.2" thickBot="1">
       <c r="B6" s="11" t="s">
@@ -1159,61 +1231,61 @@
       </c>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="21">
-      <c r="B11" s="1" t="s">
+    <row r="9" spans="2:11">
+      <c r="B9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="21">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="15.6">
-      <c r="B12" s="9"/>
-      <c r="C12" s="10" t="s">
+    <row r="13" spans="2:11" ht="15.6">
+      <c r="B13" s="9"/>
+      <c r="C13" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D13" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="37"/>
-    </row>
-    <row r="13" spans="2:11" ht="16.2" thickBot="1">
-      <c r="B13" s="11" t="s">
+      <c r="E13" s="31"/>
+    </row>
+    <row r="14" spans="2:11" ht="16.2" thickBot="1">
+      <c r="B14" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E14" s="12" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11">
-      <c r="B14" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" spans="2:11">
       <c r="B15" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="8" t="s">
@@ -1224,416 +1296,522 @@
       </c>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11">
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-    </row>
-    <row r="18" spans="2:11" ht="15.6">
-      <c r="B18" s="9"/>
-      <c r="C18" s="10" t="s">
+      <c r="C17" s="15"/>
+      <c r="D17" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="2:7" ht="15.6">
+      <c r="B19" s="9"/>
+      <c r="C19" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="37"/>
-      <c r="F18" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="37"/>
-    </row>
-    <row r="19" spans="2:11" ht="16.2" thickBot="1">
-      <c r="B19" s="11" t="s">
+      <c r="D19" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="31"/>
+      <c r="F19" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="31"/>
+    </row>
+    <row r="20" spans="2:7" ht="16.2" thickBot="1">
+      <c r="B20" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D20" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E20" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F20" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G20" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:11">
-      <c r="B20" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11">
+    <row r="21" spans="2:7">
       <c r="B21" s="13" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="23" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>41</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
       <c r="B22" s="13" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11">
-      <c r="B23" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="21">
+      <c r="B29" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="16.2" thickBot="1">
+      <c r="B30" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="21"/>
+      <c r="D30" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="38"/>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="40"/>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="42"/>
+    </row>
+    <row r="35" spans="1:11" ht="21">
+      <c r="B35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+    </row>
+    <row r="36" spans="1:11" ht="15.6">
+      <c r="B36" s="9"/>
+      <c r="C36" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" ht="21">
-      <c r="B26" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" ht="16.2" thickBot="1">
-      <c r="B27" s="20" t="s">
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="I36" s="31"/>
+      <c r="J36" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="K36" s="33"/>
+    </row>
+    <row r="37" spans="1:11" ht="15.6">
+      <c r="B37" s="22"/>
+      <c r="C37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="33"/>
+      <c r="F37" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="33"/>
+      <c r="H37" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="33"/>
+      <c r="J37" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="K37" s="33"/>
+    </row>
+    <row r="38" spans="1:11" ht="16.2" thickBot="1">
+      <c r="B38" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="41" t="s">
+      <c r="C38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="42"/>
-    </row>
-    <row r="28" spans="2:11">
-      <c r="B28" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" s="44"/>
-    </row>
-    <row r="29" spans="2:11">
-      <c r="B29" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="46"/>
-    </row>
-    <row r="32" spans="2:11" ht="21">
-      <c r="B32" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-    </row>
-    <row r="33" spans="1:11" ht="15.6">
-      <c r="B33" s="9"/>
-      <c r="C33" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="I33" s="37"/>
-      <c r="J33" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="K33" s="28"/>
-    </row>
-    <row r="34" spans="1:11" ht="15.6">
-      <c r="B34" s="22"/>
-      <c r="C34" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="28"/>
-      <c r="F34" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="G34" s="28"/>
-      <c r="H34" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="I34" s="28"/>
-      <c r="J34" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="K34" s="28"/>
-    </row>
-    <row r="35" spans="1:11" ht="16.2" thickBot="1">
-      <c r="B35" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" s="12" t="s">
+      <c r="G38" s="45"/>
+      <c r="H38" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="I38" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" s="33"/>
-      <c r="H35" s="26" t="s">
+      <c r="J38" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="I35" s="12" t="s">
+      <c r="K38" s="12" t="s">
         <v>5</v>
-      </c>
-      <c r="J35" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="B36" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F36" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="G36" s="35"/>
-      <c r="H36" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="J36" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="K36" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="B37" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F37" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="G37" s="28"/>
-      <c r="H37" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="J37" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K37" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="B38" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F38" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="G38" s="28"/>
-      <c r="H38" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="J38" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="K38" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="B39" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="G39" s="28"/>
+      <c r="E39" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F39" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" s="47"/>
       <c r="H39" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J39" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="K39" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="B40" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F40" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="G40" s="33"/>
+      <c r="H40" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="I40" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="I39" s="7" t="s">
+      <c r="J40" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="J39" s="23" t="s">
+      <c r="K40" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="K39" s="7" t="s">
+    </row>
+    <row r="41" spans="1:11">
+      <c r="B41" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" s="34" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="6"/>
-      <c r="B40" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E40" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="F40" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="G40" s="30"/>
-      <c r="H40" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="I40" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="J40" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="K40" s="19" t="s">
+      <c r="G41" s="33"/>
+      <c r="H41" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J41" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="B42" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="G42" s="33"/>
+      <c r="H42" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J42" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="K42" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="B43" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F43" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="G43" s="33"/>
+      <c r="H43" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="I43" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="J43" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="K43" s="28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="B44" s="27" t="s">
         <v>75</v>
       </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F44" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" s="33"/>
+      <c r="H44" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="I44" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="J44" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="K44" s="28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="6"/>
+      <c r="B45" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="D45" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" s="49"/>
+      <c r="H45" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I45" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="J45" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="K45" s="19" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
+  <mergeCells count="23">
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="F39:G39"/>
     <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="H36:I36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="72" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="41" max="16383" man="1"/>
+    <brk id="46" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>